<commit_message>
Added 2 scenarios for login feature
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B279C50-4971-45CC-8C82-DD10AA84ED02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82F63BC-4B4A-45F9-984B-AF94B89316E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Email</t>
   </si>
@@ -80,18 +80,9 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Books</t>
-  </si>
-  <si>
     <t>SearchText</t>
   </si>
   <si>
-    <t xml:space="preserve">The Alchemist By Coelho, Paulo </t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/</t>
-  </si>
-  <si>
     <t>Mode</t>
   </si>
   <si>
@@ -174,6 +165,9 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_NitroX_015</t>
+  </si>
+  <si>
+    <t>https://test-nitrox.altono.app/</t>
   </si>
 </sst>
 </file>
@@ -646,7 +640,7 @@
         <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -747,24 +741,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267BEEC3-E8D7-4A00-995A-DD78123AA385}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.54296875" customWidth="1"/>
-    <col min="2" max="2" width="24.36328125" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.1796875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="6" max="6" width="27.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
@@ -775,19 +768,13 @@
       <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -795,19 +782,13 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -816,12 +797,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -832,11 +813,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{1D9350A4-C0F3-4BB6-8E90-A4366ABD7E45}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -844,7 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46395AEB-19CB-45CC-8486-E417E53344FA}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -858,103 +836,103 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>33</v>
-      </c>
-      <c r="J1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added scenario for invalid login
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82F63BC-4B4A-45F9-984B-AF94B89316E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDF07FE-41F2-41A7-B191-48151C053664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Email</t>
   </si>
@@ -26,148 +26,157 @@
     <t>Testcase1</t>
   </si>
   <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>ReplaceFN</t>
+  </si>
+  <si>
+    <t>ReplaceLN</t>
+  </si>
+  <si>
+    <t>ReplaceEmail</t>
+  </si>
+  <si>
+    <t>ReplacePassword</t>
+  </si>
+  <si>
+    <t>TestFN_UNIQUE</t>
+  </si>
+  <si>
+    <t>password@123</t>
+  </si>
+  <si>
+    <t>TestLN_UNIQUE</t>
+  </si>
+  <si>
+    <t>Testcase2</t>
+  </si>
+  <si>
+    <t>password@543</t>
+  </si>
+  <si>
+    <t>sample_UNIQUE</t>
+  </si>
+  <si>
+    <t>sample+UNIQUE@townsqd.com</t>
+  </si>
+  <si>
+    <t>test+UNIQUE@townsqd.com</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>SearchText</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>TradingAccount</t>
+  </si>
+  <si>
+    <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>Spot</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Quote</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>OrderType</t>
+  </si>
+  <si>
+    <t>DealRef</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_001</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_002</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_003</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_004</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_005</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_006</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_007</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_008</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_009</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_010</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_011</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_012</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_013</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_014</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_015</t>
+  </si>
+  <si>
+    <t>https://test-nitrox.altono.app/</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>wrong password</t>
+  </si>
+  <si>
+    <t>user does not exist</t>
+  </si>
+  <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>TestData</t>
-  </si>
-  <si>
-    <t>ReplaceFN</t>
-  </si>
-  <si>
-    <t>ReplaceLN</t>
-  </si>
-  <si>
-    <t>ReplaceEmail</t>
-  </si>
-  <si>
-    <t>ReplacePassword</t>
-  </si>
-  <si>
-    <t>TestFN_UNIQUE</t>
-  </si>
-  <si>
-    <t>password@123</t>
-  </si>
-  <si>
-    <t>TestLN_UNIQUE</t>
-  </si>
-  <si>
-    <t>Testcase2</t>
-  </si>
-  <si>
-    <t>password@543</t>
-  </si>
-  <si>
-    <t>sample_UNIQUE</t>
-  </si>
-  <si>
-    <t>sample+UNIQUE@townsqd.com</t>
-  </si>
-  <si>
-    <t>test+UNIQUE@townsqd.com</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>SearchText</t>
-  </si>
-  <si>
-    <t>Mode</t>
-  </si>
-  <si>
-    <t>TradingAccount</t>
-  </si>
-  <si>
-    <t>TestCaseID</t>
-  </si>
-  <si>
-    <t>Spot</t>
-  </si>
-  <si>
-    <t>Base</t>
-  </si>
-  <si>
-    <t>Quote</t>
-  </si>
-  <si>
-    <t>Balance</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Random</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>OrderType</t>
-  </si>
-  <si>
-    <t>DealRef</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_001</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_002</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_003</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_004</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_005</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_006</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_007</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_008</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_009</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_010</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_011</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_012</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_013</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_014</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_NitroX_015</t>
-  </si>
-  <si>
-    <t>https://test-nitrox.altono.app/</t>
   </si>
 </sst>
 </file>
@@ -622,25 +631,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -684,19 +693,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -704,33 +713,33 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -741,10 +750,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267BEEC3-E8D7-4A00-995A-DD78123AA385}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -752,63 +761,76 @@
     <col min="1" max="1" width="29.54296875" customWidth="1"/>
     <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -836,103 +858,103 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>32</v>
-      </c>
-      <c r="L1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logic to take screenshot after each cucumber test step
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097005AC-5C89-465E-BE91-EFBD13E03408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E5CA41-4627-49E4-A7BB-C7CE33D0CAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="320" yWindow="2030" windowWidth="14400" windowHeight="7360" tabRatio="555" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267BEEC3-E8D7-4A00-995A-DD78123AA385}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46395AEB-19CB-45CC-8486-E417E53344FA}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added the 9 and 10 Test Case and steps
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86987C60-5898-4A25-A2CB-C525390ED16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1240B1-00E5-4144-B584-18E7C40ACBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="58">
   <si>
     <t>Email</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>Trader01@Tinyex</t>
-  </si>
-  <si>
-    <t>Trader02@Tinyex</t>
   </si>
 </sst>
 </file>
@@ -300,7 +297,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -309,9 +306,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -889,14 +883,14 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:L8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.81640625" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.6328125" customWidth="1"/>
     <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1173,8 +1167,8 @@
       <c r="B8" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>58</v>
+      <c r="C8" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>52</v>
@@ -1231,10 +1225,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C8" r:id="rId1" display="mailto:Trader02@Tinyex" xr:uid="{D0F9E5EC-B5F6-4D36-A4F7-6C102433F031}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Base and Quote Feature and NitroHome Action Class
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E226883E-5C5F-477D-8A7F-DD4294FC65A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FF8B3D-509B-4072-85F1-F463E810D5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="60">
   <si>
     <t>Email</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>Trader01@Tinyex</t>
+  </si>
+  <si>
+    <t>USDT</t>
+  </si>
+  <si>
+    <t>ETH</t>
   </si>
 </sst>
 </file>
@@ -297,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -306,6 +312,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -883,7 +892,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1192,9 +1201,42 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added The 12th Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A91E379-5C8A-4D5B-B22C-D8962E6286FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B07ABF-7C32-4824-BB1C-60050F0F938D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t>Email</t>
   </si>
@@ -898,7 +898,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1107,10 +1107,18 @@
       <c r="A10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>

</xml_diff>

<commit_message>
Implemented logic to skip step definitions based on parameter given in testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B07ABF-7C32-4824-BB1C-60050F0F938D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E367FB4-484A-464B-A99D-C85095ADB49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <si>
     <t>Email</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>--</t>
+  </si>
+  <si>
+    <t>SIT</t>
+  </si>
+  <si>
+    <t>SkipAtStepNum</t>
   </si>
 </sst>
 </file>
@@ -306,7 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -322,6 +328,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -895,10 +907,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46395AEB-19CB-45CC-8486-E417E53344FA}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -907,47 +919,54 @@
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="23.6328125" customWidth="1"/>
     <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
@@ -966,8 +985,12 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M2" s="10"/>
+      <c r="N2" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
@@ -984,8 +1007,12 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M3" s="10"/>
+      <c r="N3" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>38</v>
       </c>
@@ -1002,8 +1029,12 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M4" s="10"/>
+      <c r="N4" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>39</v>
       </c>
@@ -1020,8 +1051,12 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M5" s="10"/>
+      <c r="N5" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>40</v>
       </c>
@@ -1040,8 +1075,12 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M6" s="10"/>
+      <c r="N6" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
         <v>41</v>
       </c>
@@ -1058,8 +1097,12 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M7" s="10"/>
+      <c r="N7" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
@@ -1078,8 +1121,12 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M8" s="10"/>
+      <c r="N8" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
@@ -1102,8 +1149,12 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M9" s="10"/>
+      <c r="N9" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
         <v>44</v>
       </c>
@@ -1126,8 +1177,12 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M10" s="11"/>
+      <c r="N10" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>45</v>
       </c>
@@ -1142,8 +1197,12 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M11" s="10"/>
+      <c r="N11" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
         <v>46</v>
       </c>
@@ -1158,8 +1217,12 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M12" s="10"/>
+      <c r="N12" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="7" t="s">
         <v>47</v>
       </c>
@@ -1174,6 +1237,10 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="7" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Added 13th Test Case in feature file,steps and Home Page
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E367FB4-484A-464B-A99D-C85095ADB49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03700AEF-DAC3-4893-8649-63E080DE4E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
   <si>
     <t>Email</t>
   </si>
@@ -910,7 +910,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:L11"/>
+      <selection activeCell="B11" sqref="B11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1186,15 +1186,25 @@
       <c r="A11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="J11" s="7">
+        <v>1</v>
+      </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="10"/>
@@ -1206,15 +1216,25 @@
       <c r="A12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="J12" s="7">
+        <v>1</v>
+      </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="10"/>

</xml_diff>

<commit_message>
change in cancel order locators
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C7317A-7963-4547-996F-1FA7C2082786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2FE6F1-6B0F-47C2-9B31-3F1D52272BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -315,7 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -334,12 +334,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -919,7 +913,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -995,11 +989,11 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="J2" s="11"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="10"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
       <c r="O2" s="7" t="b">
         <v>0</v>
       </c>
@@ -1018,11 +1012,11 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="J3" s="11"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="10"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
       <c r="O3" s="7" t="b">
         <v>0</v>
       </c>
@@ -1041,11 +1035,11 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="J4" s="11"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="10"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
       <c r="O4" s="7" t="b">
         <v>0</v>
       </c>
@@ -1064,11 +1058,11 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="10"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
       <c r="O5" s="7" t="b">
         <v>0</v>
       </c>
@@ -1089,11 +1083,11 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="10"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
       <c r="O6" s="7" t="b">
         <v>0</v>
       </c>
@@ -1112,11 +1106,11 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="10"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
       <c r="O7" s="7" t="b">
         <v>0</v>
       </c>
@@ -1137,11 +1131,11 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="J8" s="11"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="10"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
       <c r="O8" s="7" t="b">
         <v>0</v>
       </c>
@@ -1166,11 +1160,11 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="J9" s="11"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="10"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
       <c r="O9" s="7" t="b">
         <v>0</v>
       </c>
@@ -1195,10 +1189,10 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="J10" s="11"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="12"/>
+      <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="7" t="b">
         <v>0</v>
@@ -1224,13 +1218,13 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="7">
+      <c r="J11" s="11">
         <v>1</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="10"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
       <c r="O11" s="7" t="b">
         <v>0</v>
       </c>
@@ -1255,15 +1249,15 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="7">
+      <c r="J12" s="11">
         <v>1</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
-      <c r="M12" s="13">
+      <c r="M12" s="11">
         <v>1</v>
       </c>
-      <c r="N12" s="10"/>
+      <c r="N12" s="11"/>
       <c r="O12" s="7" t="b">
         <v>0</v>
       </c>
@@ -1280,11 +1274,11 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
+      <c r="J13" s="11"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="10"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
       <c r="O13" s="7" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added The Test Case 15
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2FE6F1-6B0F-47C2-9B31-3F1D52272BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCFA204-E054-4833-B2C2-3F5C9E09D676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>Email</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>OpenOrderNumber</t>
+  </si>
+  <si>
+    <t>Side</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_015_01</t>
   </si>
 </sst>
 </file>
@@ -910,23 +916,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46395AEB-19CB-45CC-8486-E417E53344FA}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.81640625" customWidth="1"/>
+    <col min="1" max="1" width="33.26953125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="23.6328125" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.1796875" customWidth="1"/>
-    <col min="14" max="14" width="18.1796875" customWidth="1"/>
+    <col min="12" max="12" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" customWidth="1"/>
+    <col min="15" max="15" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
@@ -949,31 +955,34 @@
         <v>27</v>
       </c>
       <c r="H1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
@@ -989,16 +998,17 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="11"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="11"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="11"/>
-      <c r="O2" s="7" t="b">
+      <c r="O2" s="11"/>
+      <c r="P2" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
@@ -1012,16 +1022,17 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="11"/>
       <c r="L3" s="7"/>
-      <c r="M3" s="11"/>
+      <c r="M3" s="7"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="7" t="b">
+      <c r="O3" s="11"/>
+      <c r="P3" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>38</v>
       </c>
@@ -1035,16 +1046,17 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="11"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="11"/>
+      <c r="M4" s="7"/>
       <c r="N4" s="11"/>
-      <c r="O4" s="7" t="b">
+      <c r="O4" s="11"/>
+      <c r="P4" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>39</v>
       </c>
@@ -1058,16 +1070,17 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="11"/>
       <c r="L5" s="7"/>
-      <c r="M5" s="11"/>
+      <c r="M5" s="7"/>
       <c r="N5" s="11"/>
-      <c r="O5" s="7" t="b">
+      <c r="O5" s="11"/>
+      <c r="P5" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>40</v>
       </c>
@@ -1083,16 +1096,17 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="11"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="11"/>
+      <c r="M6" s="7"/>
       <c r="N6" s="11"/>
-      <c r="O6" s="7" t="b">
+      <c r="O6" s="11"/>
+      <c r="P6" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
         <v>41</v>
       </c>
@@ -1106,16 +1120,17 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="11"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="11"/>
+      <c r="M7" s="7"/>
       <c r="N7" s="11"/>
-      <c r="O7" s="7" t="b">
+      <c r="O7" s="11"/>
+      <c r="P7" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
@@ -1131,16 +1146,17 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="11"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="11"/>
+      <c r="M8" s="7"/>
       <c r="N8" s="11"/>
-      <c r="O8" s="7" t="b">
+      <c r="O8" s="11"/>
+      <c r="P8" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
@@ -1160,16 +1176,17 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="11"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="11"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="11"/>
-      <c r="O9" s="7" t="b">
+      <c r="O9" s="11"/>
+      <c r="P9" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
         <v>44</v>
       </c>
@@ -1189,16 +1206,17 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="11"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="11"/>
+      <c r="M10" s="7"/>
       <c r="N10" s="11"/>
-      <c r="O10" s="7" t="b">
+      <c r="O10" s="11"/>
+      <c r="P10" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>45</v>
       </c>
@@ -1218,18 +1236,19 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="11">
+      <c r="J11" s="7"/>
+      <c r="K11" s="11">
         <v>1</v>
       </c>
-      <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="11"/>
+      <c r="M11" s="7"/>
       <c r="N11" s="11"/>
-      <c r="O11" s="7" t="b">
+      <c r="O11" s="11"/>
+      <c r="P11" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
         <v>46</v>
       </c>
@@ -1249,43 +1268,87 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="11">
+      <c r="J12" s="7"/>
+      <c r="K12" s="11">
         <v>1</v>
       </c>
-      <c r="K12" s="7"/>
       <c r="L12" s="7"/>
-      <c r="M12" s="11">
+      <c r="M12" s="7"/>
+      <c r="N12" s="11">
         <v>1</v>
       </c>
-      <c r="N12" s="11"/>
-      <c r="O12" s="7" t="b">
+      <c r="O12" s="11"/>
+      <c r="P12" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="B13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="11">
+        <v>1</v>
+      </c>
       <c r="L13" s="7"/>
-      <c r="M13" s="11"/>
+      <c r="M13" s="7"/>
       <c r="N13" s="11"/>
-      <c r="O13" s="7" t="b">
+      <c r="O13" s="11"/>
+      <c r="P13" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="11">
+        <v>1</v>
+      </c>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="7" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the 15 Test Case and New Feature File and Step for BOT
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EC114B-89C6-46E2-AB69-1EF621767EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E83F8C-D287-4273-AA73-D31DFDA27144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
     <sheet name="RestAPITestData" sheetId="2" r:id="rId2"/>
     <sheet name="NitroXLogin" sheetId="6" r:id="rId3"/>
     <sheet name="NitroXHome" sheetId="7" r:id="rId4"/>
+    <sheet name="NitroXBots" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
   <si>
     <t>Email</t>
   </si>
@@ -225,6 +226,9 @@
   </si>
   <si>
     <t>Sell</t>
+  </si>
+  <si>
+    <t>BUY</t>
   </si>
 </sst>
 </file>
@@ -330,14 +334,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -352,9 +355,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -832,10 +832,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267BEEC3-E8D7-4A00-995A-DD78123AA385}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -845,9 +845,11 @@
     <col min="3" max="3" width="14.1796875" customWidth="1"/>
     <col min="4" max="4" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -863,15 +865,21 @@
       <c r="E1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" t="s">
         <v>53</v>
       </c>
       <c r="D2" t="s">
@@ -880,12 +888,16 @@
       <c r="E2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="10"/>
+      <c r="G2" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C3" t="s">
@@ -897,15 +909,19 @@
       <c r="E3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="10"/>
+      <c r="G3" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" t="s">
         <v>53</v>
       </c>
       <c r="D4" t="s">
@@ -913,6 +929,10 @@
       </c>
       <c r="E4" t="s">
         <v>50</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="6" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -922,7 +942,7 @@
     <hyperlink ref="C4" r:id="rId2" display="http://system.qa/" xr:uid="{9FF3C947-A236-4922-8378-3DD5674E76CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -930,9 +950,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46395AEB-19CB-45CC-8486-E417E53344FA}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5:O15"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -946,450 +966,454 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="7" t="b">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="7" t="b">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="7" t="b">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="7" t="b">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="7" t="b">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="7" t="b">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="7" t="b">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="7" t="b">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="7" t="b">
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="11">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="10">
         <v>1</v>
       </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="7" t="b">
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="11">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="10">
         <v>1</v>
       </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="11">
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="10">
         <v>1</v>
       </c>
-      <c r="O12" s="11"/>
-      <c r="P12" s="7" t="b">
+      <c r="O12" s="10"/>
+      <c r="P12" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="11">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="10">
         <v>1</v>
       </c>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="7" t="b">
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="11">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="10">
         <v>1</v>
       </c>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="7" t="b">
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7" t="s">
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="11">
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="10">
         <v>1</v>
       </c>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="7" t="b">
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1401,4 +1425,93 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" customWidth="1"/>
+    <col min="12" max="12" width="21.90625" customWidth="1"/>
+    <col min="14" max="14" width="26.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Test Case 24 Actions ,Locators and Steps and Excel Value
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D41E34B-6A9D-4E0B-8219-3BE7A0D1651A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FF2351-B893-48E0-863F-3B2AD017525D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
   <si>
     <t>Email</t>
   </si>
@@ -235,6 +235,90 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_NitroX_019</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Bot Quantity</t>
+  </si>
+  <si>
+    <t>Instrument Type</t>
+  </si>
+  <si>
+    <t>Order Direction</t>
+  </si>
+  <si>
+    <t>Min Time Break</t>
+  </si>
+  <si>
+    <t>Max Time Break</t>
+  </si>
+  <si>
+    <t>Random Range</t>
+  </si>
+  <si>
+    <t>Order Amount</t>
+  </si>
+  <si>
+    <t>Execution Strategy</t>
+  </si>
+  <si>
+    <t>Price Increment</t>
+  </si>
+  <si>
+    <t>Reserved Amount</t>
+  </si>
+  <si>
+    <t>Min Price</t>
+  </si>
+  <si>
+    <t>Max Price</t>
+  </si>
+  <si>
+    <t>Updating Break</t>
+  </si>
+  <si>
+    <t>Depth Level</t>
+  </si>
+  <si>
+    <t>Spread Benchmark</t>
+  </si>
+  <si>
+    <t>Target Altcoin</t>
+  </si>
+  <si>
+    <t>Target Quotecoin</t>
+  </si>
+  <si>
+    <t>Trigger Condition</t>
+  </si>
+  <si>
+    <t>Order Type</t>
+  </si>
+  <si>
+    <t>Stop Condition</t>
+  </si>
+  <si>
+    <t>Deal Ref</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_024</t>
+  </si>
+  <si>
+    <t>apl_bot</t>
+  </si>
+  <si>
+    <t>execution_bot</t>
+  </si>
+  <si>
+    <t>VANILLA</t>
+  </si>
+  <si>
+    <t>LIMIT</t>
   </si>
 </sst>
 </file>
@@ -956,7 +1040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46395AEB-19CB-45CC-8486-E417E53344FA}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
@@ -1503,10 +1587,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1518,7 +1602,7 @@
     <col min="14" max="14" width="26.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:34" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>22</v>
       </c>
@@ -1538,39 +1622,93 @@
         <v>26</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD1" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="9" t="s">
+      <c r="AE1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="9" t="s">
+      <c r="AF1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="AG1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="AH1" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:34" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>23</v>
@@ -1583,6 +1721,59 @@
       </c>
       <c r="E2" s="6" t="s">
         <v>58</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="6">
+        <v>15</v>
+      </c>
+      <c r="M2" s="6">
+        <v>45</v>
+      </c>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6">
+        <v>10</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6">
+        <v>3000</v>
+      </c>
+      <c r="T2" s="6">
+        <v>6000</v>
+      </c>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Locators and Actions in Bot
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FF2351-B893-48E0-863F-3B2AD017525D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816558F8-A0B9-4CD5-A389-19E59E3A3C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -424,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -445,6 +445,12 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1040,7 +1046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46395AEB-19CB-45CC-8486-E417E53344FA}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
@@ -1589,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1598,8 +1604,12 @@
     <col min="1" max="1" width="29.81640625" customWidth="1"/>
     <col min="2" max="2" width="15.26953125" customWidth="1"/>
     <col min="3" max="3" width="18.08984375" customWidth="1"/>
+    <col min="8" max="8" width="19.08984375" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.90625" customWidth="1"/>
     <col min="14" max="14" width="26.90625" customWidth="1"/>
+    <col min="33" max="33" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1706,7 +1716,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>95</v>
       </c>
@@ -1729,32 +1739,32 @@
       <c r="H2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="11">
         <v>1</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="11">
         <v>15</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="11">
         <v>45</v>
       </c>
       <c r="N2" s="6"/>
-      <c r="O2" s="6">
+      <c r="O2" s="11">
         <v>10</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="12" t="s">
         <v>98</v>
       </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
-      <c r="S2" s="6">
+      <c r="S2" s="11">
         <v>3000</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T2" s="11">
         <v>6000</v>
       </c>
       <c r="U2" s="6"/>
@@ -1778,5 +1788,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added More Action and Features in Test Case 24
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816558F8-A0B9-4CD5-A389-19E59E3A3C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4DC011-9D8C-45D0-88C2-291FC078B908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -222,9 +222,6 @@
     <t>QA_TestCase_Auto_NitroX_017</t>
   </si>
   <si>
-    <t>Trader02@Tinyex</t>
-  </si>
-  <si>
     <t>Sell</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>LIMIT</t>
+  </si>
+  <si>
+    <t>SELL</t>
   </si>
 </sst>
 </file>
@@ -1046,9 +1046,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46395AEB-19CB-45CC-8486-E417E53344FA}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1430,7 +1430,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -1464,7 +1464,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -1487,7 +1487,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>59</v>
@@ -1498,7 +1498,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -1515,13 +1515,13 @@
     </row>
     <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>59</v>
@@ -1532,7 +1532,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
@@ -1547,13 +1547,13 @@
     </row>
     <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>59</v>
@@ -1564,7 +1564,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -1581,13 +1581,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C15" r:id="rId1" xr:uid="{A7958F53-A791-4502-A04C-010F73068305}"/>
-    <hyperlink ref="C16" r:id="rId2" xr:uid="{9EF6F413-DB2F-44C2-B651-8BF4071DE32F}"/>
-    <hyperlink ref="C17" r:id="rId3" xr:uid="{E329768F-A686-4A63-800D-3E7F9FD4FB29}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1595,8 +1590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1632,73 +1627,73 @@
         <v>26</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AB1" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AC1" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="AC1" s="9" t="s">
-        <v>94</v>
       </c>
       <c r="AD1" s="9" t="s">
         <v>64</v>
@@ -1718,7 +1713,7 @@
     </row>
     <row r="2" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>23</v>
@@ -1734,30 +1729,30 @@
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" s="11">
-        <v>1</v>
+      <c r="I2" s="10">
+        <v>2</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="L2" s="11">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="M2" s="11">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N2" s="6"/>
       <c r="O2" s="11">
         <v>10</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
@@ -1774,7 +1769,7 @@
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
       <c r="AA2" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AB2" s="6"/>
       <c r="AC2" s="6"/>

</xml_diff>

<commit_message>
Test Case 24 -added  More actions and steps
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4DC011-9D8C-45D0-88C2-291FC078B908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43C877F-BE36-41AA-AE3E-2F3125F58413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="99">
   <si>
     <t>Email</t>
   </si>
@@ -316,9 +316,6 @@
   </si>
   <si>
     <t>LIMIT</t>
-  </si>
-  <si>
-    <t>SELL</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46395AEB-19CB-45CC-8486-E417E53344FA}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
@@ -1590,8 +1587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1604,6 +1601,7 @@
     <col min="10" max="10" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.90625" customWidth="1"/>
     <col min="14" max="14" width="26.90625" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1735,11 +1733,11 @@
         <v>96</v>
       </c>
       <c r="I2" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="L2" s="11">
         <v>20</v>
@@ -1749,7 +1747,7 @@
       </c>
       <c r="N2" s="6"/>
       <c r="O2" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="P2" s="12" t="s">
         <v>97</v>
@@ -1774,7 +1772,9 @@
       <c r="AB2" s="6"/>
       <c r="AC2" s="6"/>
       <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
+      <c r="AE2" s="6">
+        <v>1</v>
+      </c>
       <c r="AF2" s="6"/>
       <c r="AG2" s="6"/>
       <c r="AH2" s="6" t="b">

</xml_diff>

<commit_message>
Created Locators and reusable actions for XAlpha login feature
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8ADCCD-0CBF-43BE-976E-22B3ED7E4AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8266F7B-6701-4319-8101-043DD26B5A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="NitroXLogin" sheetId="6" r:id="rId3"/>
     <sheet name="NitroXBuySell" sheetId="7" r:id="rId4"/>
     <sheet name="NitroXBots" sheetId="8" r:id="rId5"/>
+    <sheet name="XAlphaLogin" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="103">
   <si>
     <t>Email</t>
   </si>
@@ -316,6 +317,18 @@
   </si>
   <si>
     <t>LIMIT</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_XAlpha_001</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_XAlpha_002</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_XAlpha_003</t>
+  </si>
+  <si>
+    <t>https://test-xalpha.altono.app/</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46395AEB-19CB-45CC-8486-E417E53344FA}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
@@ -1787,4 +1800,117 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD5F807-ACA8-48C4-B9BD-3C44953A349F}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="21.26953125" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="http://system.qa/" xr:uid="{901F2C83-F979-49E8-AA52-87DE6C722F75}"/>
+    <hyperlink ref="C4" r:id="rId2" display="http://system.qa/" xr:uid="{07FF1E63-0166-4347-A0BC-723A3C38F8A0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test Case 24 all steps added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8266F7B-6701-4319-8101-043DD26B5A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26BD2EA-E927-456A-B246-E4F48A7407FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -1602,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1773,7 +1773,7 @@
         <v>3000</v>
       </c>
       <c r="T2" s="11">
-        <v>6000</v>
+        <v>4000</v>
       </c>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
@@ -1806,7 +1806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD5F807-ACA8-48C4-B9BD-3C44953A349F}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added the Test Case 25
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2C7069-7821-4E3F-B8D9-6F52DFBD9C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8887B25-0150-4ABF-9C8E-A5ED0B4D554B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="555" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="105">
   <si>
     <t>Email</t>
   </si>
@@ -329,12 +329,21 @@
   </si>
   <si>
     <t>https://test-xalpha.altono.app/</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_025</t>
+  </si>
+  <si>
+    <t>SELL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -460,6 +469,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1600,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1614,6 +1626,7 @@
     <col min="8" max="8" width="19.08984375" customWidth="1"/>
     <col min="9" max="9" width="15.81640625" customWidth="1"/>
     <col min="10" max="10" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.90625" customWidth="1"/>
     <col min="14" max="14" width="26.90625" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
@@ -1761,8 +1774,8 @@
         <v>50</v>
       </c>
       <c r="N2" s="6"/>
-      <c r="O2" s="11">
-        <v>1</v>
+      <c r="O2" s="13">
+        <v>1E-3</v>
       </c>
       <c r="P2" s="12" t="s">
         <v>97</v>
@@ -1793,6 +1806,78 @@
       <c r="AF2" s="6"/>
       <c r="AG2" s="6"/>
       <c r="AH2" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="10">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="L3" s="11">
+        <v>20</v>
+      </c>
+      <c r="M3" s="11">
+        <v>50</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="11">
+        <v>3000</v>
+      </c>
+      <c r="T3" s="11">
+        <v>4000</v>
+      </c>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 25 Test Case
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8887B25-0150-4ABF-9C8E-A5ED0B4D554B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95310225-0C02-4905-8A6A-129925D85F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,7 +344,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +365,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -443,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -474,6 +480,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1614,8 +1621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
   <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1836,7 +1843,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6"/>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="14" t="s">
         <v>104</v>
       </c>
       <c r="L3" s="11">

</xml_diff>

<commit_message>
Created Pagefactory Package and added locators for test case number25
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95310225-0C02-4905-8A6A-129925D85F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A16B98-7C42-451F-943D-1C0A331F81DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,7 +344,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,12 +365,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <color rgb="FF202124"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -449,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -480,7 +474,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -974,7 +967,7 @@
     <col min="7" max="7" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1622,7 +1615,7 @@
   <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1843,7 +1836,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6"/>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="6" t="s">
         <v>104</v>
       </c>
       <c r="L3" s="11">
@@ -1862,10 +1855,10 @@
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="11">
-        <v>3000</v>
+        <v>3100</v>
       </c>
       <c r="T3" s="11">
-        <v>4000</v>
+        <v>3900</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>

</xml_diff>

<commit_message>
Added Test Case no.26 and Steps ,feature file and locator for same
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A16B98-7C42-451F-943D-1C0A331F81DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097CCEE9-3731-425C-AD35-6FBB0240E380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="555" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="107">
   <si>
     <t>Email</t>
   </si>
@@ -335,6 +335,12 @@
   </si>
   <si>
     <t>SELL</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_026</t>
+  </si>
+  <si>
+    <t>sniper_bot</t>
   </si>
 </sst>
 </file>
@@ -1612,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1878,6 +1884,36 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Test Case No 26 Snipper Bot
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA2777D-A4D2-43FA-B406-AD6365AEED02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC083E5-EA67-4E07-AA0F-D6C222E76729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="644" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="126">
   <si>
     <t>Email</t>
   </si>
@@ -387,14 +387,27 @@
   </si>
   <si>
     <t>confirmed</t>
+  </si>
+  <si>
+    <t>TotalAmount</t>
+  </si>
+  <si>
+    <t>MinPrice</t>
+  </si>
+  <si>
+    <t>MaxPrice</t>
+  </si>
+  <si>
+    <t>MaxSlippageThreshold</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -495,7 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -517,14 +530,29 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1664,10 +1692,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
-  <dimension ref="A1:AH4"/>
+  <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1682,284 +1710,344 @@
     <col min="12" max="12" width="21.90625" customWidth="1"/>
     <col min="14" max="14" width="26.90625" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:38" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AE1" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF1" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG1" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH1" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="AI1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AJ1" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AK1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AL1" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="13">
         <v>1</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="14">
         <v>20</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="14">
         <v>50</v>
       </c>
-      <c r="N2" s="6"/>
-      <c r="O2" s="13">
+      <c r="N2" s="12"/>
+      <c r="O2" s="15">
         <v>1E-3</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="11">
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="14">
         <v>3000</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="14">
         <v>4000</v>
       </c>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6" t="s">
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6">
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12">
         <v>1</v>
       </c>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="6" t="s">
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="13">
         <v>1</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6" t="s">
+      <c r="J3" s="12"/>
+      <c r="K3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="14">
         <v>20</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="14">
         <v>50</v>
       </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="13">
+      <c r="N3" s="12"/>
+      <c r="O3" s="15">
         <v>1E-3</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="11">
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="14">
         <v>3100</v>
       </c>
-      <c r="T3" s="11">
+      <c r="T3" s="14">
         <v>3900</v>
       </c>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6" t="s">
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6">
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="12"/>
+      <c r="AE3" s="12"/>
+      <c r="AF3" s="12"/>
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="12"/>
+      <c r="AI3" s="12">
         <v>1</v>
       </c>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="6" t="s">
+      <c r="AJ3" s="12"/>
+      <c r="AK3" s="12"/>
+      <c r="AL3" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="13">
         <v>1</v>
       </c>
-      <c r="AG4" s="6"/>
-      <c r="AH4" s="6" t="b">
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE4" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="AF4" s="17">
+        <v>3000</v>
+      </c>
+      <c r="AG4" s="17">
+        <v>4000</v>
+      </c>
+      <c r="AH4" s="17">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2086,8 +2174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added test case no27
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC083E5-EA67-4E07-AA0F-D6C222E76729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076283F4-5DE2-4687-8AB9-CF1B65FE8A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="644" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="130">
   <si>
     <t>Email</t>
   </si>
@@ -399,6 +399,18 @@
   </si>
   <si>
     <t>MaxSlippageThreshold</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snipper Bot </t>
+  </si>
+  <si>
+    <t>Indicator</t>
+  </si>
+  <si>
+    <t>Bot</t>
   </si>
 </sst>
 </file>
@@ -432,7 +444,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,6 +460,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,7 +526,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -554,6 +572,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1692,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
-  <dimension ref="A1:AL4"/>
+  <dimension ref="A1:AN5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AE6" sqref="AE6"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AG12" sqref="AG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1713,9 +1738,10 @@
     <col min="31" max="31" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="19.90625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>22</v>
       </c>
@@ -1803,19 +1829,19 @@
       <c r="AC1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AD1" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AE1" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AF1" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AG1" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AH1" s="19" t="s">
         <v>125</v>
       </c>
       <c r="AI1" s="11" t="s">
@@ -1830,8 +1856,14 @@
       <c r="AL1" s="11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="AM1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AN1" s="20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>94</v>
       </c>
@@ -1906,8 +1938,12 @@
       <c r="AL2" s="12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="AM2" s="21"/>
+      <c r="AN2" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>103</v>
       </c>
@@ -1982,8 +2018,10 @@
       <c r="AL3" s="12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>105</v>
       </c>
@@ -2050,6 +2088,78 @@
       <c r="AL4" s="12" t="b">
         <v>0</v>
       </c>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" s="13">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE5" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="AF5" s="17">
+        <v>3000</v>
+      </c>
+      <c r="AG5" s="17">
+        <v>4000</v>
+      </c>
+      <c r="AH5" s="17">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added 5 assertion points in QA-TestCase-Auto-X-Alpha-004()
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076283F4-5DE2-4687-8AB9-CF1B65FE8A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8F6AF8-5A30-4DA3-A5E8-C1F9618D58BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="644" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="131">
   <si>
     <t>Email</t>
   </si>
@@ -380,9 +380,6 @@
     <t>BTC</t>
   </si>
   <si>
-    <t>processed</t>
-  </si>
-  <si>
     <t>Joejoe Pen</t>
   </si>
   <si>
@@ -411,6 +408,12 @@
   </si>
   <si>
     <t>Bot</t>
+  </si>
+  <si>
+    <t>DealType</t>
+  </si>
+  <si>
+    <t>FX Spot</t>
   </si>
 </sst>
 </file>
@@ -1719,7 +1722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
   <dimension ref="A1:AN5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+    <sheetView topLeftCell="X1" workbookViewId="0">
       <selection activeCell="AG12" sqref="AG12"/>
     </sheetView>
   </sheetViews>
@@ -1833,16 +1836,16 @@
         <v>64</v>
       </c>
       <c r="AE1" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF1" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AG1" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AH1" s="19" t="s">
         <v>124</v>
-      </c>
-      <c r="AH1" s="19" t="s">
-        <v>125</v>
       </c>
       <c r="AI1" s="11" t="s">
         <v>30</v>
@@ -1857,10 +1860,10 @@
         <v>61</v>
       </c>
       <c r="AM1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN1" s="20" t="s">
         <v>128</v>
-      </c>
-      <c r="AN1" s="20" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.35">
@@ -1940,7 +1943,7 @@
       </c>
       <c r="AM2" s="21"/>
       <c r="AN2" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.35">
@@ -2093,7 +2096,7 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>23</v>
@@ -2284,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2298,25 +2301,25 @@
         <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" t="s">
         <v>107</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>108</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>109</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>110</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>111</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>112</v>
-      </c>
-      <c r="H1" t="s">
-        <v>113</v>
       </c>
       <c r="I1" t="s">
         <v>114</v>
@@ -2339,34 +2342,34 @@
         <v>116</v>
       </c>
       <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
         <v>117</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>118</v>
-      </c>
-      <c r="E2" t="s">
-        <v>58</v>
       </c>
       <c r="F2" t="s">
         <v>58</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>119</v>
-      </c>
-      <c r="I2" t="s">
-        <v>120</v>
       </c>
       <c r="J2">
         <v>8000</v>
       </c>
       <c r="K2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N2" s="6" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added direction assertion in QA_TestCase_Auto_X-Alpha_004
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8F6AF8-5A30-4DA3-A5E8-C1F9618D58BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C37F4D1-56A6-4DE6-BDC0-2EB06AC5CE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2288,7 +2288,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Moved dealsEnquiry actions to a new class
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C37F4D1-56A6-4DE6-BDC0-2EB06AC5CE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B321E9-9848-4EA4-8784-BD9F09ADE0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="133">
   <si>
     <t>Email</t>
   </si>
@@ -374,9 +374,6 @@
     <t>QA_TestCase_Auto_X-Alpha_004</t>
   </si>
   <si>
-    <t>Buy</t>
-  </si>
-  <si>
     <t>BTC</t>
   </si>
   <si>
@@ -414,6 +411,15 @@
   </si>
   <si>
     <t>FX Spot</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_X-Alpha_005</t>
+  </si>
+  <si>
+    <t>sell</t>
+  </si>
+  <si>
+    <t>buy</t>
   </si>
 </sst>
 </file>
@@ -1836,16 +1842,16 @@
         <v>64</v>
       </c>
       <c r="AE1" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF1" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AG1" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AH1" s="19" t="s">
         <v>123</v>
-      </c>
-      <c r="AH1" s="19" t="s">
-        <v>124</v>
       </c>
       <c r="AI1" s="11" t="s">
         <v>30</v>
@@ -1860,10 +1866,10 @@
         <v>61</v>
       </c>
       <c r="AM1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN1" s="20" t="s">
         <v>127</v>
-      </c>
-      <c r="AN1" s="20" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.35">
@@ -1943,7 +1949,7 @@
       </c>
       <c r="AM2" s="21"/>
       <c r="AN2" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.35">
@@ -2096,7 +2102,7 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>23</v>
@@ -2285,15 +2291,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2301,7 +2314,7 @@
         <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C1" t="s">
         <v>107</v>
@@ -2342,16 +2355,16 @@
         <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
         <v>58</v>
@@ -2363,15 +2376,53 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J2">
         <v>8000</v>
       </c>
       <c r="K2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N2" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3">
+        <v>8000</v>
+      </c>
+      <c r="K3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N3" s="6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Segregated test data files w.r.t. app name
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5438E4FB-985C-406F-B578-C39FCF30EF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9625D0E-CE6F-49EA-905A-05EBB8A9DB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="5" r:id="rId1"/>
@@ -13,15 +13,13 @@
     <sheet name="NitroXLogin" sheetId="6" r:id="rId3"/>
     <sheet name="NitroXBuySell" sheetId="7" r:id="rId4"/>
     <sheet name="NitroXBots" sheetId="8" r:id="rId5"/>
-    <sheet name="XAlphaLogin" sheetId="9" r:id="rId6"/>
-    <sheet name="XAlphaDeals" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="111">
   <si>
     <t>Email</t>
   </si>
@@ -320,18 +318,6 @@
     <t>LIMIT</t>
   </si>
   <si>
-    <t>QA_TestCase_Auto_XAlpha_001</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_XAlpha_002</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_XAlpha_003</t>
-  </si>
-  <si>
-    <t>https://test-xalpha.altono.app/</t>
-  </si>
-  <si>
     <t>QA_TestCase_Auto_NitroX_025</t>
   </si>
   <si>
@@ -344,45 +330,6 @@
     <t>sniper_bot</t>
   </si>
   <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>BaseAssetAmount</t>
-  </si>
-  <si>
-    <t>BaseAsset</t>
-  </si>
-  <si>
-    <t>QuoteAsset</t>
-  </si>
-  <si>
-    <t>FeeAsset</t>
-  </si>
-  <si>
-    <t>FeeAmount</t>
-  </si>
-  <si>
-    <t>ProcessingStatus</t>
-  </si>
-  <si>
-    <t>CounterpartyName</t>
-  </si>
-  <si>
-    <t>PortfolioNumber</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_X-Alpha_004</t>
-  </si>
-  <si>
-    <t>BTC</t>
-  </si>
-  <si>
-    <t>Joejoe Pen</t>
-  </si>
-  <si>
-    <t>confirmed</t>
-  </si>
-  <si>
     <t>TotalAmount</t>
   </si>
   <si>
@@ -405,27 +352,6 @@
   </si>
   <si>
     <t>Bot</t>
-  </si>
-  <si>
-    <t>DealType</t>
-  </si>
-  <si>
-    <t>FX Spot</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_X-Alpha_005</t>
-  </si>
-  <si>
-    <t>buy</t>
-  </si>
-  <si>
-    <t>pending</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_X-Alpha_006</t>
-  </si>
-  <si>
-    <t>processed</t>
   </si>
 </sst>
 </file>
@@ -1734,8 +1660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F12E04-623E-4AA8-BAE7-FE646A9FB65C}">
   <dimension ref="A1:AN5"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AG12" sqref="AG12"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AF9" sqref="AF9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1848,16 +1774,16 @@
         <v>64</v>
       </c>
       <c r="AE1" s="19" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="AF1" s="19" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="AG1" s="19" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="AH1" s="19" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="AI1" s="11" t="s">
         <v>30</v>
@@ -1872,10 +1798,10 @@
         <v>61</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="AN1" s="20" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.35">
@@ -1955,12 +1881,12 @@
       </c>
       <c r="AM2" s="21"/>
       <c r="AN2" s="2" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>23</v>
@@ -1986,7 +1912,7 @@
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L3" s="14">
         <v>20</v>
@@ -2038,7 +1964,7 @@
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>23</v>
@@ -2057,7 +1983,7 @@
         <v>95</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -2108,7 +2034,7 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>23</v>
@@ -2127,7 +2053,7 @@
         <v>95</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I5" s="13">
         <v>1</v>
@@ -2153,7 +2079,7 @@
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AE5" s="18">
         <v>0.1</v>
@@ -2180,297 +2106,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD5F807-ACA8-48C4-B9BD-3C44953A349F}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="29.54296875" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" customWidth="1"/>
-    <col min="6" max="6" width="16.1796875" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://system.qa/" xr:uid="{901F2C83-F979-49E8-AA52-87DE6C722F75}"/>
-    <hyperlink ref="C4" r:id="rId2" display="http://system.qa/" xr:uid="{07FF1E63-0166-4347-A0BC-723A3C38F8A0}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
-  <dimension ref="A1:N4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K1" t="s">
-        <v>113</v>
-      </c>
-      <c r="M1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>118</v>
-      </c>
-      <c r="J2">
-        <v>8000</v>
-      </c>
-      <c r="K2" t="s">
-        <v>119</v>
-      </c>
-      <c r="N2" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J3">
-        <v>8000</v>
-      </c>
-      <c r="K3" t="s">
-        <v>132</v>
-      </c>
-      <c r="N3" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>118</v>
-      </c>
-      <c r="J4">
-        <v>8000</v>
-      </c>
-      <c r="K4" t="s">
-        <v>134</v>
-      </c>
-      <c r="N4" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>